<commit_message>
modificacio archivo excel cotizacion
modificado
</commit_message>
<xml_diff>
--- a/RUMISOFT2019/RUMISOFT/bin/Debug/formato/COTIZACION.xlsx
+++ b/RUMISOFT2019/RUMISOFT/bin/Debug/formato/COTIZACION.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SISTEMA ZITRO\RUMISOFT2019\RUMISOFT\bin\Debug\formato\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\ZITROSOFT\RUMISOFT2019\RUMISOFT\bin\Debug\formato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE7CE52-157A-4B54-8B1E-FA8B5876BDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083B0235-16F4-4AE0-BA35-519105F2C573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -688,98 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -787,6 +696,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -802,11 +714,99 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:E26"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1226,50 +1226,50 @@
     </row>
     <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
     </row>
     <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -1282,10 +1282,10 @@
       <c r="L8" s="37"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="39"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="37"/>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -1298,10 +1298,10 @@
       <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
@@ -1314,10 +1314,10 @@
       <c r="L10" s="37"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -1330,10 +1330,10 @@
       <c r="L11" s="37"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="39"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
@@ -1346,10 +1346,10 @@
       <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="39"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
@@ -1362,203 +1362,206 @@
       <c r="L13" s="37"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="38" t="s">
+      <c r="B14" s="50"/>
+      <c r="C14" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
-      <c r="L17" s="79"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="49"/>
     </row>
     <row r="18" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="28"/>
       <c r="G18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="72"/>
     </row>
     <row r="19" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="27"/>
       <c r="G19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="46"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="70"/>
     </row>
     <row r="20" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="76"/>
       <c r="F20" s="29"/>
       <c r="G20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="50"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="74"/>
     </row>
     <row r="21" spans="1:12" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="26"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="70"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="39"/>
     </row>
     <row r="22" spans="1:12" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="55" t="s">
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="55" t="s">
+      <c r="G22" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="55" t="s">
+      <c r="H22" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="55" t="s">
+      <c r="J22" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="55" t="s">
+      <c r="K22" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="55" t="s">
+      <c r="L22" s="42" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="72"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:12" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="81"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="54"/>
       <c r="F24" s="18"/>
       <c r="G24" s="17"/>
       <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="I24" s="18">
+        <f>C16/100</f>
+        <v>0</v>
+      </c>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="81"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
       <c r="F25" s="18"/>
       <c r="G25" s="17"/>
       <c r="H25" s="18"/>
@@ -1569,10 +1572,10 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="81"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="18"/>
       <c r="G26" s="17"/>
       <c r="H26" s="18"/>
@@ -1583,10 +1586,10 @@
     </row>
     <row r="27" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="81"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="18"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
@@ -1597,10 +1600,10 @@
     </row>
     <row r="28" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="81"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="18"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
@@ -1611,10 +1614,10 @@
     </row>
     <row r="29" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="81"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
       <c r="F29" s="18"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
@@ -1625,10 +1628,10 @@
     </row>
     <row r="30" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="81"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
       <c r="F30" s="18"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
@@ -1639,10 +1642,10 @@
     </row>
     <row r="31" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="81"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="54"/>
       <c r="F31" s="18"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
@@ -1653,10 +1656,10 @@
     </row>
     <row r="32" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="81"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="54"/>
       <c r="F32" s="18"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
@@ -1667,10 +1670,10 @@
     </row>
     <row r="33" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="81"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="54"/>
       <c r="F33" s="18"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
@@ -1681,10 +1684,10 @@
     </row>
     <row r="34" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="81"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="54"/>
       <c r="F34" s="18"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
@@ -1695,10 +1698,10 @@
     </row>
     <row r="35" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="81"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="54"/>
       <c r="F35" s="18"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
@@ -1709,10 +1712,10 @@
     </row>
     <row r="36" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="81"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="54"/>
       <c r="F36" s="18"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
@@ -1723,10 +1726,10 @@
     </row>
     <row r="37" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="81"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="54"/>
       <c r="F37" s="18"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
@@ -1737,10 +1740,10 @@
     </row>
     <row r="38" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="16"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="81"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="54"/>
       <c r="F38" s="18"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
@@ -1751,10 +1754,10 @@
     </row>
     <row r="39" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="81"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="54"/>
       <c r="F39" s="18"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
@@ -1765,10 +1768,10 @@
     </row>
     <row r="40" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="16"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="81"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="54"/>
       <c r="F40" s="18"/>
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
@@ -1779,10 +1782,10 @@
     </row>
     <row r="41" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="81"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
       <c r="F41" s="18"/>
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
@@ -1793,10 +1796,10 @@
     </row>
     <row r="42" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="81"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="54"/>
       <c r="F42" s="18"/>
       <c r="G42" s="17"/>
       <c r="H42" s="20"/>
@@ -1807,10 +1810,10 @@
     </row>
     <row r="43" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="81"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="54"/>
       <c r="F43" s="18"/>
       <c r="G43" s="17"/>
       <c r="H43" s="18"/>
@@ -1884,20 +1887,20 @@
       <c r="L47" s="34"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="58" t="s">
+      <c r="A48" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="59"/>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="60"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="59"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
@@ -1909,8 +1912,8 @@
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
-      <c r="K49" s="67"/>
-      <c r="L49" s="68"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="67"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
@@ -1920,8 +1923,8 @@
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="62"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="61"/>
     </row>
     <row r="51" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
@@ -1933,8 +1936,8 @@
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="65"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="64"/>
     </row>
     <row r="52" spans="1:12" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
@@ -2002,52 +2005,52 @@
       <c r="A58" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
       <c r="G58" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
-      <c r="K58" s="67"/>
-      <c r="L58" s="68"/>
+      <c r="K58" s="66"/>
+      <c r="L58" s="67"/>
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="66"/>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="65"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
-      <c r="K59" s="61"/>
-      <c r="L59" s="62"/>
+      <c r="K59" s="60"/>
+      <c r="L59" s="61"/>
     </row>
     <row r="60" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="69"/>
-      <c r="C60" s="69"/>
-      <c r="D60" s="69"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="68"/>
       <c r="G60" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
-      <c r="K60" s="64"/>
-      <c r="L60" s="65"/>
+      <c r="K60" s="63"/>
+      <c r="L60" s="64"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="56"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
+      <c r="A61" s="55"/>
+      <c r="B61" s="56"/>
+      <c r="C61" s="56"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -2060,63 +2063,6 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C13:L13"/>
-    <mergeCell ref="G21:L21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="B22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:L16"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C7:L7"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="A14:B14"/>
@@ -2133,6 +2079,63 @@
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="C12:L12"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="C13:L13"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="B22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>